<commit_message>
deleted bom.csv and positions.csv in the production files
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ludwin/Elektronik/rotating_sphere/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB37D96-0061-F442-840B-CBEA7C254889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B8AC1C-AACA-1B42-ABBC-20A5C400BC4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="680" windowWidth="28240" windowHeight="16980" xr2:uid="{C5747C83-2E8F-6F4A-BB98-C4FF20A52BD6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>BOM Rotating Sphere</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>Amazon, ebay, others</t>
+  </si>
+  <si>
+    <t>DC motor 31ZY, 6V, 4000rpm</t>
+  </si>
+  <si>
+    <t>https://amzn.eu/d/0FNWCg7</t>
   </si>
 </sst>
 </file>
@@ -497,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{961A1468-A0F2-D241-B3A1-C6C4EE62311E}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection sqref="A1:E12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -646,6 +652,23 @@
         <v>18</v>
       </c>
     </row>
+    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D9" r:id="rId1" xr:uid="{8546801D-8CD4-E646-8708-2D8E147322E9}"/>

</xml_diff>